<commit_message>
push login feature with invalid data
</commit_message>
<xml_diff>
--- a/Data Files/Login Data.xlsx
+++ b/Data Files/Login Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\git\Automation-openRMS\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E6FEC1-8F10-4A31-8ED2-C19679FA23A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763B8BCA-C9A5-4BB6-9B3C-1925213A3CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{002CBD15-2C30-496C-85A2-1A54428D15E2}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7270" xr2:uid="{002CBD15-2C30-496C-85A2-1A54428D15E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Location" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,6 @@
     <t>TD001</t>
   </si>
   <si>
-    <t>Inpatiant Ward</t>
-  </si>
-  <si>
     <t>Isolation Ward</t>
   </si>
   <si>
@@ -78,13 +75,16 @@
   </si>
   <si>
     <t>TD006</t>
+  </si>
+  <si>
+    <t>Inpatient Ward</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -466,15 +466,15 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -482,52 +482,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>